<commit_message>
balancing, ninjaboy: dash and straight shot
</commit_message>
<xml_diff>
--- a/balancing/balancing.xlsx
+++ b/balancing/balancing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Sutter\Documents\HSLU\BeautifulBullets\balancing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC43103-CDA7-40AF-987A-D881DF66B406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4E3092-84DA-4943-955C-DA4533F3A5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2A03D44-C4D6-4004-94B0-83E0462C7539}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>Yoimiya</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Ninja Boy</t>
   </si>
   <si>
-    <t>Nabil</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -174,6 +171,48 @@
   </si>
   <si>
     <t>bps</t>
+  </si>
+  <si>
+    <t>shiftspeed</t>
+  </si>
+  <si>
+    <t>ninja boy kill in sec</t>
+  </si>
+  <si>
+    <t>yoimiya kill in sec</t>
+  </si>
+  <si>
+    <t>1000 damage done in sec</t>
+  </si>
+  <si>
+    <t>bulletspeed</t>
+  </si>
+  <si>
+    <t>Challenger Ability</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>passive charge speed</t>
+  </si>
+  <si>
+    <t>grace charge speed</t>
+  </si>
+  <si>
+    <t>charge required</t>
+  </si>
+  <si>
+    <t>Machine Gun Bow</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>straight shot</t>
   </si>
 </sst>
 </file>
@@ -543,11 +582,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J48"/>
+  <dimension ref="A2:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="117" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C47" sqref="C47"/>
+      <selection pane="topRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,17 +599,17 @@
     <col min="11" max="11" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -578,104 +617,83 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>3000</v>
+        <v>1100</v>
       </c>
       <c r="D6" s="2">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1000</v>
-      </c>
+        <v>800</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2">
-        <v>80</v>
-      </c>
-      <c r="E7" s="2">
-        <v>50</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E7" s="2"/>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
       </c>
       <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2">
         <v>2.5</v>
       </c>
+      <c r="E8" s="2"/>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2">
         <v>55</v>
@@ -691,12 +709,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -712,9 +730,9 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2">
         <v>10</v>
@@ -730,9 +748,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="2">
         <f>C11/C12</f>
@@ -752,64 +770,64 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -819,13 +837,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2"/>
       <c r="H19" s="2"/>
@@ -833,7 +851,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -845,10 +863,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2">
         <v>3</v>
@@ -860,7 +878,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2">
         <v>10</v>
@@ -872,19 +890,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2">
         <f>C20/C21</f>
@@ -903,67 +921,80 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="2">
         <v>45</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2">
         <v>10</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2">
         <v>10</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2">
+        <v>10</v>
+      </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="2">
         <f>C27/C28</f>
         <v>4.5</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2">
+        <f>D27/D28</f>
+        <v>2</v>
+      </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -973,10 +1004,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -984,20 +1015,20 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" s="2">
         <v>5</v>
@@ -1007,7 +1038,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="2">
         <v>10</v>
@@ -1017,7 +1048,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2">
         <v>8</v>
@@ -1027,7 +1058,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38" s="2">
         <v>75</v>
@@ -1037,12 +1068,12 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -1050,13 +1081,10 @@
       <c r="D42" t="s">
         <v>1</v>
       </c>
-      <c r="E42" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -1064,31 +1092,182 @@
       <c r="D44">
         <v>2</v>
       </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>1.3</v>
+      </c>
+      <c r="D45">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46">
         <v>8</v>
       </c>
-      <c r="B46" t="s">
-        <v>11</v>
+      <c r="D46">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D48">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49">
+        <v>1.3</v>
+      </c>
+      <c r="D49">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51">
+        <v>1.5</v>
+      </c>
+      <c r="D51">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53">
+        <f>1000/C47/C48</f>
+        <v>36.231884057971016</v>
+      </c>
+      <c r="D53">
+        <f>1000/D47/D48</f>
+        <v>29.239766081871341</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55">
+        <f>$C6/C47/C48</f>
+        <v>39.855072463768124</v>
+      </c>
+      <c r="D55">
+        <f>$C6/D47/D48</f>
+        <v>32.163742690058477</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56">
+        <f>$D6/C47/C48</f>
+        <v>28.985507246376816</v>
+      </c>
+      <c r="D56">
+        <f>$D6/D47/D48</f>
+        <v>23.391812865497077</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>